<commit_message>
descripción de las columnas del df
</commit_message>
<xml_diff>
--- a/descripcion_columnas.xlsx
+++ b/descripcion_columnas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0eaf3dded534d368/Desktop/Data_Analytics/pairprogramming/da-modulo3-sprint2-pairprogramming-RocioZahara/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{1EFE7357-562F-46DD-9809-4328A1AE8E71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="14_{1EFE7357-562F-46DD-9809-4328A1AE8E71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D50B6EC7-E690-41AB-9108-B7B6AC0256BE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B6AD6A28-098F-4BCB-B9B1-38D4DF1DBB96}"/>
   </bookViews>
@@ -765,10 +765,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1072,7 +1068,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>